<commit_message>
updated app config files
</commit_message>
<xml_diff>
--- a/Email_Reporter/ReportSpreadsheet.xlsx
+++ b/Email_Reporter/ReportSpreadsheet.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="940" yWindow="80" windowWidth="25600" windowHeight="14560"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WebParserReport" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UnitTestReport" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="WebParserReport" sheetId="1" r:id="rId1"/>
+    <sheet name="UnitTestReport" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>2017-12-12</t>
   </si>
   <si>
     <t>Old_Data</t>
@@ -47,36 +49,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,17 +93,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -427,67 +430,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="3">
+        <v>43070</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -496,10 +496,15 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>